<commit_message>
removed stuff added stuff
</commit_message>
<xml_diff>
--- a/stock_predictor_ai/data/cleaned/PYPL.xlsx
+++ b/stock_predictor_ai/data/cleaned/PYPL.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2509"/>
+  <dimension ref="A1:F2566"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -39948,7 +39948,7 @@
         <v>72.95999908447266</v>
       </c>
       <c r="F1975" t="n">
-        <v>11941800</v>
+        <v>11954200</v>
       </c>
     </row>
     <row r="1976">
@@ -40048,7 +40048,7 @@
         <v>64.09999847412109</v>
       </c>
       <c r="F1980" t="n">
-        <v>28654300</v>
+        <v>28711100</v>
       </c>
     </row>
     <row r="1981">
@@ -40148,7 +40148,7 @@
         <v>61.90000152587891</v>
       </c>
       <c r="F1985" t="n">
-        <v>19362800</v>
+        <v>19398000</v>
       </c>
     </row>
     <row r="1986">
@@ -40328,7 +40328,7 @@
         <v>63.7400016784668</v>
       </c>
       <c r="F1994" t="n">
-        <v>16423200</v>
+        <v>16438700</v>
       </c>
     </row>
     <row r="1995">
@@ -40428,7 +40428,7 @@
         <v>64</v>
       </c>
       <c r="F1999" t="n">
-        <v>17140800</v>
+        <v>17151700</v>
       </c>
     </row>
     <row r="2000">
@@ -40528,7 +40528,7 @@
         <v>65.94999694824219</v>
       </c>
       <c r="F2004" t="n">
-        <v>29690500</v>
+        <v>29703700</v>
       </c>
     </row>
     <row r="2005">
@@ -40608,7 +40608,7 @@
         <v>67.41500091552734</v>
       </c>
       <c r="F2008" t="n">
-        <v>27616200</v>
+        <v>27683800</v>
       </c>
     </row>
     <row r="2009">
@@ -40708,7 +40708,7 @@
         <v>66.08999633789062</v>
       </c>
       <c r="F2013" t="n">
-        <v>16894000</v>
+        <v>16907100</v>
       </c>
     </row>
     <row r="2014">
@@ -40788,7 +40788,7 @@
         <v>66.19000244140625</v>
       </c>
       <c r="F2017" t="n">
-        <v>12313900</v>
+        <v>12341800</v>
       </c>
     </row>
     <row r="2018">
@@ -40888,7 +40888,7 @@
         <v>72.66000366210938</v>
       </c>
       <c r="F2022" t="n">
-        <v>12192500</v>
+        <v>12202200</v>
       </c>
     </row>
     <row r="2023">
@@ -40928,7 +40928,7 @@
         <v>73.48000335693359</v>
       </c>
       <c r="F2024" t="n">
-        <v>11915000</v>
+        <v>11903000</v>
       </c>
     </row>
     <row r="2025">
@@ -40988,7 +40988,7 @@
         <v>72.73000335693359</v>
       </c>
       <c r="F2027" t="n">
-        <v>25508500</v>
+        <v>25515000</v>
       </c>
     </row>
     <row r="2028">
@@ -41188,7 +41188,7 @@
         <v>64.80000305175781</v>
       </c>
       <c r="F2037" t="n">
-        <v>25230100</v>
+        <v>25279500</v>
       </c>
     </row>
     <row r="2038">
@@ -41288,7 +41288,7 @@
         <v>62.27000045776367</v>
       </c>
       <c r="F2042" t="n">
-        <v>12393700</v>
+        <v>12419300</v>
       </c>
     </row>
     <row r="2043">
@@ -41388,7 +41388,7 @@
         <v>57.38999938964844</v>
       </c>
       <c r="F2047" t="n">
-        <v>19020500</v>
+        <v>19035900</v>
       </c>
     </row>
     <row r="2048">
@@ -41428,7 +41428,7 @@
         <v>59.91999816894531</v>
       </c>
       <c r="F2049" t="n">
-        <v>17364200</v>
+        <v>17340200</v>
       </c>
     </row>
     <row r="2050">
@@ -41588,7 +41588,7 @@
         <v>63.13000106811523</v>
       </c>
       <c r="F2057" t="n">
-        <v>11709600</v>
+        <v>11715200</v>
       </c>
     </row>
     <row r="2058">
@@ -41768,7 +41768,7 @@
         <v>64.66000366210938</v>
       </c>
       <c r="F2066" t="n">
-        <v>21818700</v>
+        <v>21843500</v>
       </c>
     </row>
     <row r="2067">
@@ -41848,7 +41848,7 @@
         <v>59.95000076293945</v>
       </c>
       <c r="F2070" t="n">
-        <v>15343900</v>
+        <v>15361000</v>
       </c>
     </row>
     <row r="2071">
@@ -41968,7 +41968,7 @@
         <v>58.84999847412109</v>
       </c>
       <c r="F2076" t="n">
-        <v>10544900</v>
+        <v>10550300</v>
       </c>
     </row>
     <row r="2077">
@@ -42068,7 +42068,7 @@
         <v>56.83000183105469</v>
       </c>
       <c r="F2081" t="n">
-        <v>18344500</v>
+        <v>18348600</v>
       </c>
     </row>
     <row r="2082">
@@ -42268,7 +42268,7 @@
         <v>53.9900016784668</v>
       </c>
       <c r="F2091" t="n">
-        <v>20966100</v>
+        <v>20982500</v>
       </c>
     </row>
     <row r="2092">
@@ -42468,7 +42468,7 @@
         <v>55.41999816894531</v>
       </c>
       <c r="F2101" t="n">
-        <v>18722400</v>
+        <v>18742100</v>
       </c>
     </row>
     <row r="2102">
@@ -42848,7 +42848,7 @@
         <v>57.63000106811523</v>
       </c>
       <c r="F2120" t="n">
-        <v>18416900</v>
+        <v>18435700</v>
       </c>
     </row>
     <row r="2121">
@@ -42948,7 +42948,7 @@
         <v>58.2599983215332</v>
       </c>
       <c r="F2125" t="n">
-        <v>15458300</v>
+        <v>15467500</v>
       </c>
     </row>
     <row r="2126">
@@ -43048,7 +43048,7 @@
         <v>62.36999893188477</v>
       </c>
       <c r="F2130" t="n">
-        <v>23996000</v>
+        <v>24011000</v>
       </c>
     </row>
     <row r="2131">
@@ -43148,7 +43148,7 @@
         <v>62.16999816894531</v>
       </c>
       <c r="F2135" t="n">
-        <v>13164000</v>
+        <v>13175400</v>
       </c>
     </row>
     <row r="2136">
@@ -43228,7 +43228,7 @@
         <v>63</v>
       </c>
       <c r="F2139" t="n">
-        <v>16779000</v>
+        <v>16807400</v>
       </c>
     </row>
     <row r="2140">
@@ -43308,7 +43308,7 @@
         <v>57.7400016784668</v>
       </c>
       <c r="F2143" t="n">
-        <v>17413600</v>
+        <v>17420200</v>
       </c>
     </row>
     <row r="2144">
@@ -43408,7 +43408,7 @@
         <v>61.79999923706055</v>
       </c>
       <c r="F2148" t="n">
-        <v>9275600</v>
+        <v>9282600</v>
       </c>
     </row>
     <row r="2149">
@@ -43488,7 +43488,7 @@
         <v>63</v>
       </c>
       <c r="F2152" t="n">
-        <v>37995100</v>
+        <v>38264600</v>
       </c>
     </row>
     <row r="2153">
@@ -43688,7 +43688,7 @@
         <v>61.79000091552734</v>
       </c>
       <c r="F2162" t="n">
-        <v>14611700</v>
+        <v>14618900</v>
       </c>
     </row>
     <row r="2163">
@@ -43888,7 +43888,7 @@
         <v>58.86000061035156</v>
       </c>
       <c r="F2172" t="n">
-        <v>12181800</v>
+        <v>12195800</v>
       </c>
     </row>
     <row r="2173">
@@ -43928,7 +43928,7 @@
         <v>58.08000183105469</v>
       </c>
       <c r="F2174" t="n">
-        <v>13424300</v>
+        <v>13377900</v>
       </c>
     </row>
     <row r="2175">
@@ -44068,7 +44068,7 @@
         <v>60.52999877929688</v>
       </c>
       <c r="F2181" t="n">
-        <v>17462600</v>
+        <v>17590400</v>
       </c>
     </row>
     <row r="2182">
@@ -44168,7 +44168,7 @@
         <v>58.72000122070312</v>
       </c>
       <c r="F2186" t="n">
-        <v>18272400</v>
+        <v>18283500</v>
       </c>
     </row>
     <row r="2187">
@@ -44268,7 +44268,7 @@
         <v>62.59999847412109</v>
       </c>
       <c r="F2191" t="n">
-        <v>20032000</v>
+        <v>20040000</v>
       </c>
     </row>
     <row r="2192">
@@ -44368,7 +44368,7 @@
         <v>66.44000244140625</v>
       </c>
       <c r="F2196" t="n">
-        <v>10196000</v>
+        <v>10208100</v>
       </c>
     </row>
     <row r="2197">
@@ -44548,7 +44548,7 @@
         <v>64.69999694824219</v>
       </c>
       <c r="F2205" t="n">
-        <v>8058000</v>
+        <v>8062300</v>
       </c>
     </row>
     <row r="2206">
@@ -44588,7 +44588,7 @@
         <v>66.94999694824219</v>
       </c>
       <c r="F2207" t="n">
-        <v>8459900</v>
+        <v>8446300</v>
       </c>
     </row>
     <row r="2208">
@@ -44648,7 +44648,7 @@
         <v>65.37999725341797</v>
       </c>
       <c r="F2210" t="n">
-        <v>9909200</v>
+        <v>9934000</v>
       </c>
     </row>
     <row r="2211">
@@ -44748,7 +44748,7 @@
         <v>62</v>
       </c>
       <c r="F2215" t="n">
-        <v>13118800</v>
+        <v>13177900</v>
       </c>
     </row>
     <row r="2216">
@@ -45248,7 +45248,7 @@
         <v>61.95000076293945</v>
       </c>
       <c r="F2240" t="n">
-        <v>8171300</v>
+        <v>8176800</v>
       </c>
     </row>
     <row r="2241">
@@ -45308,7 +45308,7 @@
         <v>62.77000045776367</v>
       </c>
       <c r="F2243" t="n">
-        <v>11874700</v>
+        <v>11867500</v>
       </c>
     </row>
     <row r="2244">
@@ -45448,7 +45448,7 @@
         <v>66.97000122070312</v>
       </c>
       <c r="F2250" t="n">
-        <v>11978800</v>
+        <v>11972300</v>
       </c>
     </row>
     <row r="2251">
@@ -45608,7 +45608,7 @@
         <v>59.91999816894531</v>
       </c>
       <c r="F2258" t="n">
-        <v>18888300</v>
+        <v>18848700</v>
       </c>
     </row>
     <row r="2259">
@@ -45648,7 +45648,7 @@
         <v>59.56999969482422</v>
       </c>
       <c r="F2260" t="n">
-        <v>9359200</v>
+        <v>9248800</v>
       </c>
     </row>
     <row r="2261">
@@ -46748,7 +46748,7 @@
         <v>69.13999938964844</v>
       </c>
       <c r="F2315" t="n">
-        <v>8376700</v>
+        <v>8369100</v>
       </c>
     </row>
     <row r="2316">
@@ -47688,7 +47688,7 @@
         <v>86.05500030517578</v>
       </c>
       <c r="F2362" t="n">
-        <v>10152600</v>
+        <v>10148100</v>
       </c>
     </row>
     <row r="2363">
@@ -48668,7 +48668,7 @@
         <v>89.56999969482422</v>
       </c>
       <c r="F2411" t="n">
-        <v>8338900</v>
+        <v>8331400</v>
       </c>
     </row>
     <row r="2412">
@@ -50288,7 +50288,7 @@
         <v>72.16000366210938</v>
       </c>
       <c r="F2492" t="n">
-        <v>7058900</v>
+        <v>7058300</v>
       </c>
     </row>
     <row r="2493">
@@ -50628,7 +50628,1147 @@
         <v>73.125</v>
       </c>
       <c r="F2509" t="n">
-        <v>9494500</v>
+        <v>9500900</v>
+      </c>
+    </row>
+    <row r="2510">
+      <c r="A2510" s="2" t="n">
+        <v>45833</v>
+      </c>
+      <c r="B2510" t="n">
+        <v>73.06999969482422</v>
+      </c>
+      <c r="C2510" t="n">
+        <v>74.25</v>
+      </c>
+      <c r="D2510" t="n">
+        <v>72.41500091552734</v>
+      </c>
+      <c r="E2510" t="n">
+        <v>74.13999938964844</v>
+      </c>
+      <c r="F2510" t="n">
+        <v>7851900</v>
+      </c>
+    </row>
+    <row r="2511">
+      <c r="A2511" s="2" t="n">
+        <v>45834</v>
+      </c>
+      <c r="B2511" t="n">
+        <v>73.16999816894531</v>
+      </c>
+      <c r="C2511" t="n">
+        <v>73.37999725341797</v>
+      </c>
+      <c r="D2511" t="n">
+        <v>71.61000061035156</v>
+      </c>
+      <c r="E2511" t="n">
+        <v>73.24500274658203</v>
+      </c>
+      <c r="F2511" t="n">
+        <v>10235600</v>
+      </c>
+    </row>
+    <row r="2512">
+      <c r="A2512" s="2" t="n">
+        <v>45835</v>
+      </c>
+      <c r="B2512" t="n">
+        <v>73.63999938964844</v>
+      </c>
+      <c r="C2512" t="n">
+        <v>73.75</v>
+      </c>
+      <c r="D2512" t="n">
+        <v>72.85500335693359</v>
+      </c>
+      <c r="E2512" t="n">
+        <v>73.26999664306641</v>
+      </c>
+      <c r="F2512" t="n">
+        <v>10449500</v>
+      </c>
+    </row>
+    <row r="2513">
+      <c r="A2513" s="2" t="n">
+        <v>45838</v>
+      </c>
+      <c r="B2513" t="n">
+        <v>74.31999969482422</v>
+      </c>
+      <c r="C2513" t="n">
+        <v>74.54000091552734</v>
+      </c>
+      <c r="D2513" t="n">
+        <v>73.66000366210938</v>
+      </c>
+      <c r="E2513" t="n">
+        <v>73.94000244140625</v>
+      </c>
+      <c r="F2513" t="n">
+        <v>7738000</v>
+      </c>
+    </row>
+    <row r="2514">
+      <c r="A2514" s="2" t="n">
+        <v>45839</v>
+      </c>
+      <c r="B2514" t="n">
+        <v>75.29000091552734</v>
+      </c>
+      <c r="C2514" t="n">
+        <v>75.69499969482422</v>
+      </c>
+      <c r="D2514" t="n">
+        <v>73.80000305175781</v>
+      </c>
+      <c r="E2514" t="n">
+        <v>73.94999694824219</v>
+      </c>
+      <c r="F2514" t="n">
+        <v>8633800</v>
+      </c>
+    </row>
+    <row r="2515">
+      <c r="A2515" s="2" t="n">
+        <v>45840</v>
+      </c>
+      <c r="B2515" t="n">
+        <v>76.30999755859375</v>
+      </c>
+      <c r="C2515" t="n">
+        <v>76.86499786376953</v>
+      </c>
+      <c r="D2515" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2515" t="n">
+        <v>75.01000213623047</v>
+      </c>
+      <c r="F2515" t="n">
+        <v>9361500</v>
+      </c>
+    </row>
+    <row r="2516">
+      <c r="A2516" s="2" t="n">
+        <v>45841</v>
+      </c>
+      <c r="B2516" t="n">
+        <v>76.58999633789062</v>
+      </c>
+      <c r="C2516" t="n">
+        <v>77.36000061035156</v>
+      </c>
+      <c r="D2516" t="n">
+        <v>76.47499847412109</v>
+      </c>
+      <c r="E2516" t="n">
+        <v>76.70999908447266</v>
+      </c>
+      <c r="F2516" t="n">
+        <v>5263400</v>
+      </c>
+    </row>
+    <row r="2517">
+      <c r="A2517" s="2" t="n">
+        <v>45845</v>
+      </c>
+      <c r="B2517" t="n">
+        <v>76.18000030517578</v>
+      </c>
+      <c r="C2517" t="n">
+        <v>76.83000183105469</v>
+      </c>
+      <c r="D2517" t="n">
+        <v>75.62000274658203</v>
+      </c>
+      <c r="E2517" t="n">
+        <v>76.20999908447266</v>
+      </c>
+      <c r="F2517" t="n">
+        <v>5918600</v>
+      </c>
+    </row>
+    <row r="2518">
+      <c r="A2518" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="B2518" t="n">
+        <v>75.02999877929688</v>
+      </c>
+      <c r="C2518" t="n">
+        <v>76.51499938964844</v>
+      </c>
+      <c r="D2518" t="n">
+        <v>74.51000213623047</v>
+      </c>
+      <c r="E2518" t="n">
+        <v>76.44000244140625</v>
+      </c>
+      <c r="F2518" t="n">
+        <v>8758400</v>
+      </c>
+    </row>
+    <row r="2519">
+      <c r="A2519" s="2" t="n">
+        <v>45847</v>
+      </c>
+      <c r="B2519" t="n">
+        <v>74.83000183105469</v>
+      </c>
+      <c r="C2519" t="n">
+        <v>75.79000091552734</v>
+      </c>
+      <c r="D2519" t="n">
+        <v>74.375</v>
+      </c>
+      <c r="E2519" t="n">
+        <v>75.48999786376953</v>
+      </c>
+      <c r="F2519" t="n">
+        <v>6755700</v>
+      </c>
+    </row>
+    <row r="2520">
+      <c r="A2520" s="2" t="n">
+        <v>45848</v>
+      </c>
+      <c r="B2520" t="n">
+        <v>75.69999694824219</v>
+      </c>
+      <c r="C2520" t="n">
+        <v>76.22000122070312</v>
+      </c>
+      <c r="D2520" t="n">
+        <v>74.12999725341797</v>
+      </c>
+      <c r="E2520" t="n">
+        <v>74.45500183105469</v>
+      </c>
+      <c r="F2520" t="n">
+        <v>6380200</v>
+      </c>
+    </row>
+    <row r="2521">
+      <c r="A2521" s="2" t="n">
+        <v>45849</v>
+      </c>
+      <c r="B2521" t="n">
+        <v>71.36000061035156</v>
+      </c>
+      <c r="C2521" t="n">
+        <v>75.19999694824219</v>
+      </c>
+      <c r="D2521" t="n">
+        <v>70.79000091552734</v>
+      </c>
+      <c r="E2521" t="n">
+        <v>75.16999816894531</v>
+      </c>
+      <c r="F2521" t="n">
+        <v>21877700</v>
+      </c>
+    </row>
+    <row r="2522">
+      <c r="A2522" s="2" t="n">
+        <v>45852</v>
+      </c>
+      <c r="B2522" t="n">
+        <v>73.88999938964844</v>
+      </c>
+      <c r="C2522" t="n">
+        <v>74.30999755859375</v>
+      </c>
+      <c r="D2522" t="n">
+        <v>71.54000091552734</v>
+      </c>
+      <c r="E2522" t="n">
+        <v>71.55999755859375</v>
+      </c>
+      <c r="F2522" t="n">
+        <v>12993900</v>
+      </c>
+    </row>
+    <row r="2523">
+      <c r="A2523" s="2" t="n">
+        <v>45853</v>
+      </c>
+      <c r="B2523" t="n">
+        <v>72.95999908447266</v>
+      </c>
+      <c r="C2523" t="n">
+        <v>73.91000366210938</v>
+      </c>
+      <c r="D2523" t="n">
+        <v>72.94000244140625</v>
+      </c>
+      <c r="E2523" t="n">
+        <v>73.76999664306641</v>
+      </c>
+      <c r="F2523" t="n">
+        <v>7333600</v>
+      </c>
+    </row>
+    <row r="2524">
+      <c r="A2524" s="2" t="n">
+        <v>45854</v>
+      </c>
+      <c r="B2524" t="n">
+        <v>72.97000122070312</v>
+      </c>
+      <c r="C2524" t="n">
+        <v>73.58000183105469</v>
+      </c>
+      <c r="D2524" t="n">
+        <v>71.73000335693359</v>
+      </c>
+      <c r="E2524" t="n">
+        <v>73.26000213623047</v>
+      </c>
+      <c r="F2524" t="n">
+        <v>9671100</v>
+      </c>
+    </row>
+    <row r="2525">
+      <c r="A2525" s="2" t="n">
+        <v>45855</v>
+      </c>
+      <c r="B2525" t="n">
+        <v>73.86000061035156</v>
+      </c>
+      <c r="C2525" t="n">
+        <v>74.18000030517578</v>
+      </c>
+      <c r="D2525" t="n">
+        <v>72.34999847412109</v>
+      </c>
+      <c r="E2525" t="n">
+        <v>72.47000122070312</v>
+      </c>
+      <c r="F2525" t="n">
+        <v>8522700</v>
+      </c>
+    </row>
+    <row r="2526">
+      <c r="A2526" s="2" t="n">
+        <v>45856</v>
+      </c>
+      <c r="B2526" t="n">
+        <v>74.16999816894531</v>
+      </c>
+      <c r="C2526" t="n">
+        <v>74.34999847412109</v>
+      </c>
+      <c r="D2526" t="n">
+        <v>73.28399658203125</v>
+      </c>
+      <c r="E2526" t="n">
+        <v>74.09999847412109</v>
+      </c>
+      <c r="F2526" t="n">
+        <v>9011600</v>
+      </c>
+    </row>
+    <row r="2527">
+      <c r="A2527" s="2" t="n">
+        <v>45859</v>
+      </c>
+      <c r="B2527" t="n">
+        <v>74.81999969482422</v>
+      </c>
+      <c r="C2527" t="n">
+        <v>76.23000335693359</v>
+      </c>
+      <c r="D2527" t="n">
+        <v>74.23999786376953</v>
+      </c>
+      <c r="E2527" t="n">
+        <v>74.34999847412109</v>
+      </c>
+      <c r="F2527" t="n">
+        <v>8200400</v>
+      </c>
+    </row>
+    <row r="2528">
+      <c r="A2528" s="2" t="n">
+        <v>45860</v>
+      </c>
+      <c r="B2528" t="n">
+        <v>76</v>
+      </c>
+      <c r="C2528" t="n">
+        <v>76.15000152587891</v>
+      </c>
+      <c r="D2528" t="n">
+        <v>74.76499938964844</v>
+      </c>
+      <c r="E2528" t="n">
+        <v>74.76499938964844</v>
+      </c>
+      <c r="F2528" t="n">
+        <v>9094400</v>
+      </c>
+    </row>
+    <row r="2529">
+      <c r="A2529" s="2" t="n">
+        <v>45861</v>
+      </c>
+      <c r="B2529" t="n">
+        <v>76.66000366210938</v>
+      </c>
+      <c r="C2529" t="n">
+        <v>77.23000335693359</v>
+      </c>
+      <c r="D2529" t="n">
+        <v>75.91000366210938</v>
+      </c>
+      <c r="E2529" t="n">
+        <v>76.92500305175781</v>
+      </c>
+      <c r="F2529" t="n">
+        <v>9283200</v>
+      </c>
+    </row>
+    <row r="2530">
+      <c r="A2530" s="2" t="n">
+        <v>45862</v>
+      </c>
+      <c r="B2530" t="n">
+        <v>77.81999969482422</v>
+      </c>
+      <c r="C2530" t="n">
+        <v>78.76000213623047</v>
+      </c>
+      <c r="D2530" t="n">
+        <v>77.34999847412109</v>
+      </c>
+      <c r="E2530" t="n">
+        <v>77.73999786376953</v>
+      </c>
+      <c r="F2530" t="n">
+        <v>10504300</v>
+      </c>
+    </row>
+    <row r="2531">
+      <c r="A2531" s="2" t="n">
+        <v>45863</v>
+      </c>
+      <c r="B2531" t="n">
+        <v>77.98000335693359</v>
+      </c>
+      <c r="C2531" t="n">
+        <v>78.81500244140625</v>
+      </c>
+      <c r="D2531" t="n">
+        <v>77.5</v>
+      </c>
+      <c r="E2531" t="n">
+        <v>77.58999633789062</v>
+      </c>
+      <c r="F2531" t="n">
+        <v>6888100</v>
+      </c>
+    </row>
+    <row r="2532">
+      <c r="A2532" s="2" t="n">
+        <v>45866</v>
+      </c>
+      <c r="B2532" t="n">
+        <v>78.22000122070312</v>
+      </c>
+      <c r="C2532" t="n">
+        <v>79.5</v>
+      </c>
+      <c r="D2532" t="n">
+        <v>77.93000030517578</v>
+      </c>
+      <c r="E2532" t="n">
+        <v>78.51000213623047</v>
+      </c>
+      <c r="F2532" t="n">
+        <v>15978400</v>
+      </c>
+    </row>
+    <row r="2533">
+      <c r="A2533" s="2" t="n">
+        <v>45867</v>
+      </c>
+      <c r="B2533" t="n">
+        <v>71.44999694824219</v>
+      </c>
+      <c r="C2533" t="n">
+        <v>73.27999877929688</v>
+      </c>
+      <c r="D2533" t="n">
+        <v>70.30999755859375</v>
+      </c>
+      <c r="E2533" t="n">
+        <v>71.73000335693359</v>
+      </c>
+      <c r="F2533" t="n">
+        <v>42890700</v>
+      </c>
+    </row>
+    <row r="2534">
+      <c r="A2534" s="2" t="n">
+        <v>45868</v>
+      </c>
+      <c r="B2534" t="n">
+        <v>69.70999908447266</v>
+      </c>
+      <c r="C2534" t="n">
+        <v>72.20500183105469</v>
+      </c>
+      <c r="D2534" t="n">
+        <v>69.55500030517578</v>
+      </c>
+      <c r="E2534" t="n">
+        <v>72.19000244140625</v>
+      </c>
+      <c r="F2534" t="n">
+        <v>20790400</v>
+      </c>
+    </row>
+    <row r="2535">
+      <c r="A2535" s="2" t="n">
+        <v>45869</v>
+      </c>
+      <c r="B2535" t="n">
+        <v>68.76000213623047</v>
+      </c>
+      <c r="C2535" t="n">
+        <v>70.05500030517578</v>
+      </c>
+      <c r="D2535" t="n">
+        <v>68.45999908447266</v>
+      </c>
+      <c r="E2535" t="n">
+        <v>69.47499847412109</v>
+      </c>
+      <c r="F2535" t="n">
+        <v>16657600</v>
+      </c>
+    </row>
+    <row r="2536">
+      <c r="A2536" s="2" t="n">
+        <v>45870</v>
+      </c>
+      <c r="B2536" t="n">
+        <v>67.11000061035156</v>
+      </c>
+      <c r="C2536" t="n">
+        <v>68.34999847412109</v>
+      </c>
+      <c r="D2536" t="n">
+        <v>66.56999969482422</v>
+      </c>
+      <c r="E2536" t="n">
+        <v>68</v>
+      </c>
+      <c r="F2536" t="n">
+        <v>15181100</v>
+      </c>
+    </row>
+    <row r="2537">
+      <c r="A2537" s="2" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B2537" t="n">
+        <v>68.01000213623047</v>
+      </c>
+      <c r="C2537" t="n">
+        <v>68.56999969482422</v>
+      </c>
+      <c r="D2537" t="n">
+        <v>67.27500152587891</v>
+      </c>
+      <c r="E2537" t="n">
+        <v>67.82499694824219</v>
+      </c>
+      <c r="F2537" t="n">
+        <v>11756800</v>
+      </c>
+    </row>
+    <row r="2538">
+      <c r="A2538" s="2" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B2538" t="n">
+        <v>67.83000183105469</v>
+      </c>
+      <c r="C2538" t="n">
+        <v>68.66999816894531</v>
+      </c>
+      <c r="D2538" t="n">
+        <v>67.41000366210938</v>
+      </c>
+      <c r="E2538" t="n">
+        <v>68.45999908447266</v>
+      </c>
+      <c r="F2538" t="n">
+        <v>10714700</v>
+      </c>
+    </row>
+    <row r="2539">
+      <c r="A2539" s="2" t="n">
+        <v>45875</v>
+      </c>
+      <c r="B2539" t="n">
+        <v>69.41999816894531</v>
+      </c>
+      <c r="C2539" t="n">
+        <v>69.61000061035156</v>
+      </c>
+      <c r="D2539" t="n">
+        <v>68.20899963378906</v>
+      </c>
+      <c r="E2539" t="n">
+        <v>68.30000305175781</v>
+      </c>
+      <c r="F2539" t="n">
+        <v>11913000</v>
+      </c>
+    </row>
+    <row r="2540">
+      <c r="A2540" s="2" t="n">
+        <v>45876</v>
+      </c>
+      <c r="B2540" t="n">
+        <v>68.22000122070312</v>
+      </c>
+      <c r="C2540" t="n">
+        <v>70.16999816894531</v>
+      </c>
+      <c r="D2540" t="n">
+        <v>67.68000030517578</v>
+      </c>
+      <c r="E2540" t="n">
+        <v>70</v>
+      </c>
+      <c r="F2540" t="n">
+        <v>10129300</v>
+      </c>
+    </row>
+    <row r="2541">
+      <c r="A2541" s="2" t="n">
+        <v>45877</v>
+      </c>
+      <c r="B2541" t="n">
+        <v>67.65000152587891</v>
+      </c>
+      <c r="C2541" t="n">
+        <v>68.61000061035156</v>
+      </c>
+      <c r="D2541" t="n">
+        <v>67.41999816894531</v>
+      </c>
+      <c r="E2541" t="n">
+        <v>68.44000244140625</v>
+      </c>
+      <c r="F2541" t="n">
+        <v>9683400</v>
+      </c>
+    </row>
+    <row r="2542">
+      <c r="A2542" s="2" t="n">
+        <v>45880</v>
+      </c>
+      <c r="B2542" t="n">
+        <v>67.08000183105469</v>
+      </c>
+      <c r="C2542" t="n">
+        <v>68.48000335693359</v>
+      </c>
+      <c r="D2542" t="n">
+        <v>66.90000152587891</v>
+      </c>
+      <c r="E2542" t="n">
+        <v>67.80999755859375</v>
+      </c>
+      <c r="F2542" t="n">
+        <v>10118600</v>
+      </c>
+    </row>
+    <row r="2543">
+      <c r="A2543" s="2" t="n">
+        <v>45881</v>
+      </c>
+      <c r="B2543" t="n">
+        <v>67.97000122070312</v>
+      </c>
+      <c r="C2543" t="n">
+        <v>68.73999786376953</v>
+      </c>
+      <c r="D2543" t="n">
+        <v>67.23000335693359</v>
+      </c>
+      <c r="E2543" t="n">
+        <v>67.23999786376953</v>
+      </c>
+      <c r="F2543" t="n">
+        <v>9747500</v>
+      </c>
+    </row>
+    <row r="2544">
+      <c r="A2544" s="2" t="n">
+        <v>45882</v>
+      </c>
+      <c r="B2544" t="n">
+        <v>70.62999725341797</v>
+      </c>
+      <c r="C2544" t="n">
+        <v>70.73000335693359</v>
+      </c>
+      <c r="D2544" t="n">
+        <v>68.15000152587891</v>
+      </c>
+      <c r="E2544" t="n">
+        <v>68.23000335693359</v>
+      </c>
+      <c r="F2544" t="n">
+        <v>12344700</v>
+      </c>
+    </row>
+    <row r="2545">
+      <c r="A2545" s="2" t="n">
+        <v>45883</v>
+      </c>
+      <c r="B2545" t="n">
+        <v>69.37999725341797</v>
+      </c>
+      <c r="C2545" t="n">
+        <v>69.81999969482422</v>
+      </c>
+      <c r="D2545" t="n">
+        <v>68.23000335693359</v>
+      </c>
+      <c r="E2545" t="n">
+        <v>69.44000244140625</v>
+      </c>
+      <c r="F2545" t="n">
+        <v>10695400</v>
+      </c>
+    </row>
+    <row r="2546">
+      <c r="A2546" s="2" t="n">
+        <v>45884</v>
+      </c>
+      <c r="B2546" t="n">
+        <v>69.23000335693359</v>
+      </c>
+      <c r="C2546" t="n">
+        <v>70.16000366210938</v>
+      </c>
+      <c r="D2546" t="n">
+        <v>69.16000366210938</v>
+      </c>
+      <c r="E2546" t="n">
+        <v>69.56999969482422</v>
+      </c>
+      <c r="F2546" t="n">
+        <v>8128000</v>
+      </c>
+    </row>
+    <row r="2547">
+      <c r="A2547" s="2" t="n">
+        <v>45887</v>
+      </c>
+      <c r="B2547" t="n">
+        <v>69.52999877929688</v>
+      </c>
+      <c r="C2547" t="n">
+        <v>69.98500061035156</v>
+      </c>
+      <c r="D2547" t="n">
+        <v>69.23000335693359</v>
+      </c>
+      <c r="E2547" t="n">
+        <v>69.30999755859375</v>
+      </c>
+      <c r="F2547" t="n">
+        <v>8410200</v>
+      </c>
+    </row>
+    <row r="2548">
+      <c r="A2548" s="2" t="n">
+        <v>45888</v>
+      </c>
+      <c r="B2548" t="n">
+        <v>69.05000305175781</v>
+      </c>
+      <c r="C2548" t="n">
+        <v>70.36499786376953</v>
+      </c>
+      <c r="D2548" t="n">
+        <v>68.93000030517578</v>
+      </c>
+      <c r="E2548" t="n">
+        <v>69.79000091552734</v>
+      </c>
+      <c r="F2548" t="n">
+        <v>9052800</v>
+      </c>
+    </row>
+    <row r="2549">
+      <c r="A2549" s="2" t="n">
+        <v>45889</v>
+      </c>
+      <c r="B2549" t="n">
+        <v>68.08000183105469</v>
+      </c>
+      <c r="C2549" t="n">
+        <v>69.11000061035156</v>
+      </c>
+      <c r="D2549" t="n">
+        <v>67.68000030517578</v>
+      </c>
+      <c r="E2549" t="n">
+        <v>68.94000244140625</v>
+      </c>
+      <c r="F2549" t="n">
+        <v>9992300</v>
+      </c>
+    </row>
+    <row r="2550">
+      <c r="A2550" s="2" t="n">
+        <v>45890</v>
+      </c>
+      <c r="B2550" t="n">
+        <v>67.55000305175781</v>
+      </c>
+      <c r="C2550" t="n">
+        <v>67.87000274658203</v>
+      </c>
+      <c r="D2550" t="n">
+        <v>66.92500305175781</v>
+      </c>
+      <c r="E2550" t="n">
+        <v>67.68000030517578</v>
+      </c>
+      <c r="F2550" t="n">
+        <v>7039500</v>
+      </c>
+    </row>
+    <row r="2551">
+      <c r="A2551" s="2" t="n">
+        <v>45891</v>
+      </c>
+      <c r="B2551" t="n">
+        <v>69.90000152587891</v>
+      </c>
+      <c r="C2551" t="n">
+        <v>70.15000152587891</v>
+      </c>
+      <c r="D2551" t="n">
+        <v>67.81999969482422</v>
+      </c>
+      <c r="E2551" t="n">
+        <v>67.91000366210938</v>
+      </c>
+      <c r="F2551" t="n">
+        <v>9394100</v>
+      </c>
+    </row>
+    <row r="2552">
+      <c r="A2552" s="2" t="n">
+        <v>45894</v>
+      </c>
+      <c r="B2552" t="n">
+        <v>69.48000335693359</v>
+      </c>
+      <c r="C2552" t="n">
+        <v>69.80999755859375</v>
+      </c>
+      <c r="D2552" t="n">
+        <v>69.04000091552734</v>
+      </c>
+      <c r="E2552" t="n">
+        <v>69.65000152587891</v>
+      </c>
+      <c r="F2552" t="n">
+        <v>6460300</v>
+      </c>
+    </row>
+    <row r="2553">
+      <c r="A2553" s="2" t="n">
+        <v>45895</v>
+      </c>
+      <c r="B2553" t="n">
+        <v>70.18000030517578</v>
+      </c>
+      <c r="C2553" t="n">
+        <v>70.25</v>
+      </c>
+      <c r="D2553" t="n">
+        <v>69.18000030517578</v>
+      </c>
+      <c r="E2553" t="n">
+        <v>69.40000152587891</v>
+      </c>
+      <c r="F2553" t="n">
+        <v>9471500</v>
+      </c>
+    </row>
+    <row r="2554">
+      <c r="A2554" s="2" t="n">
+        <v>45896</v>
+      </c>
+      <c r="B2554" t="n">
+        <v>69.65000152587891</v>
+      </c>
+      <c r="C2554" t="n">
+        <v>70.08000183105469</v>
+      </c>
+      <c r="D2554" t="n">
+        <v>68.69100189208984</v>
+      </c>
+      <c r="E2554" t="n">
+        <v>68.73000335693359</v>
+      </c>
+      <c r="F2554" t="n">
+        <v>8648200</v>
+      </c>
+    </row>
+    <row r="2555">
+      <c r="A2555" s="2" t="n">
+        <v>45897</v>
+      </c>
+      <c r="B2555" t="n">
+        <v>70.05999755859375</v>
+      </c>
+      <c r="C2555" t="n">
+        <v>70.55999755859375</v>
+      </c>
+      <c r="D2555" t="n">
+        <v>69.52999877929688</v>
+      </c>
+      <c r="E2555" t="n">
+        <v>70</v>
+      </c>
+      <c r="F2555" t="n">
+        <v>5882000</v>
+      </c>
+    </row>
+    <row r="2556">
+      <c r="A2556" s="2" t="n">
+        <v>45898</v>
+      </c>
+      <c r="B2556" t="n">
+        <v>70.19000244140625</v>
+      </c>
+      <c r="C2556" t="n">
+        <v>70.69999694824219</v>
+      </c>
+      <c r="D2556" t="n">
+        <v>69.90000152587891</v>
+      </c>
+      <c r="E2556" t="n">
+        <v>70.01999664306641</v>
+      </c>
+      <c r="F2556" t="n">
+        <v>5636300</v>
+      </c>
+    </row>
+    <row r="2557">
+      <c r="A2557" s="2" t="n">
+        <v>45902</v>
+      </c>
+      <c r="B2557" t="n">
+        <v>69.25</v>
+      </c>
+      <c r="C2557" t="n">
+        <v>69.37400054931641</v>
+      </c>
+      <c r="D2557" t="n">
+        <v>68.15000152587891</v>
+      </c>
+      <c r="E2557" t="n">
+        <v>68.91999816894531</v>
+      </c>
+      <c r="F2557" t="n">
+        <v>12882500</v>
+      </c>
+    </row>
+    <row r="2558">
+      <c r="A2558" s="2" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B2558" t="n">
+        <v>69.63999938964844</v>
+      </c>
+      <c r="C2558" t="n">
+        <v>69.88999938964844</v>
+      </c>
+      <c r="D2558" t="n">
+        <v>68.80000305175781</v>
+      </c>
+      <c r="E2558" t="n">
+        <v>68.91000366210938</v>
+      </c>
+      <c r="F2558" t="n">
+        <v>11808200</v>
+      </c>
+    </row>
+    <row r="2559">
+      <c r="A2559" s="2" t="n">
+        <v>45904</v>
+      </c>
+      <c r="B2559" t="n">
+        <v>68.45999908447266</v>
+      </c>
+      <c r="C2559" t="n">
+        <v>69.90000152587891</v>
+      </c>
+      <c r="D2559" t="n">
+        <v>66.23000335693359</v>
+      </c>
+      <c r="E2559" t="n">
+        <v>69.69999694824219</v>
+      </c>
+      <c r="F2559" t="n">
+        <v>14063500</v>
+      </c>
+    </row>
+    <row r="2560">
+      <c r="A2560" s="2" t="n">
+        <v>45905</v>
+      </c>
+      <c r="B2560" t="n">
+        <v>68.26000213623047</v>
+      </c>
+      <c r="C2560" t="n">
+        <v>69.94000244140625</v>
+      </c>
+      <c r="D2560" t="n">
+        <v>68.16999816894531</v>
+      </c>
+      <c r="E2560" t="n">
+        <v>68.87999725341797</v>
+      </c>
+      <c r="F2560" t="n">
+        <v>7794300</v>
+      </c>
+    </row>
+    <row r="2561">
+      <c r="A2561" s="2" t="n">
+        <v>45908</v>
+      </c>
+      <c r="B2561" t="n">
+        <v>68.40000152587891</v>
+      </c>
+      <c r="C2561" t="n">
+        <v>68.58999633789062</v>
+      </c>
+      <c r="D2561" t="n">
+        <v>67.80000305175781</v>
+      </c>
+      <c r="E2561" t="n">
+        <v>68.45999908447266</v>
+      </c>
+      <c r="F2561" t="n">
+        <v>7954900</v>
+      </c>
+    </row>
+    <row r="2562">
+      <c r="A2562" s="2" t="n">
+        <v>45909</v>
+      </c>
+      <c r="B2562" t="n">
+        <v>67.68000030517578</v>
+      </c>
+      <c r="C2562" t="n">
+        <v>68.5</v>
+      </c>
+      <c r="D2562" t="n">
+        <v>67.52999877929688</v>
+      </c>
+      <c r="E2562" t="n">
+        <v>68.19999694824219</v>
+      </c>
+      <c r="F2562" t="n">
+        <v>8776500</v>
+      </c>
+    </row>
+    <row r="2563">
+      <c r="A2563" s="2" t="n">
+        <v>45910</v>
+      </c>
+      <c r="B2563" t="n">
+        <v>65.63999938964844</v>
+      </c>
+      <c r="C2563" t="n">
+        <v>68.02999877929688</v>
+      </c>
+      <c r="D2563" t="n">
+        <v>65.23500061035156</v>
+      </c>
+      <c r="E2563" t="n">
+        <v>67.48000335693359</v>
+      </c>
+      <c r="F2563" t="n">
+        <v>14352500</v>
+      </c>
+    </row>
+    <row r="2564">
+      <c r="A2564" s="2" t="n">
+        <v>45911</v>
+      </c>
+      <c r="B2564" t="n">
+        <v>67.26999664306641</v>
+      </c>
+      <c r="C2564" t="n">
+        <v>67.34999847412109</v>
+      </c>
+      <c r="D2564" t="n">
+        <v>65.70999908447266</v>
+      </c>
+      <c r="E2564" t="n">
+        <v>65.75</v>
+      </c>
+      <c r="F2564" t="n">
+        <v>11154400</v>
+      </c>
+    </row>
+    <row r="2565">
+      <c r="A2565" s="2" t="n">
+        <v>45912</v>
+      </c>
+      <c r="B2565" t="n">
+        <v>66.88999938964844</v>
+      </c>
+      <c r="C2565" t="n">
+        <v>67.75</v>
+      </c>
+      <c r="D2565" t="n">
+        <v>66.86000061035156</v>
+      </c>
+      <c r="E2565" t="n">
+        <v>67.20999908447266</v>
+      </c>
+      <c r="F2565" t="n">
+        <v>7498000</v>
+      </c>
+    </row>
+    <row r="2566">
+      <c r="A2566" s="2" t="n">
+        <v>45915</v>
+      </c>
+      <c r="B2566" t="n">
+        <v>67.71499633789062</v>
+      </c>
+      <c r="C2566" t="n">
+        <v>67.88999938964844</v>
+      </c>
+      <c r="D2566" t="n">
+        <v>67.25240325927734</v>
+      </c>
+      <c r="E2566" t="n">
+        <v>67.26999664306641</v>
+      </c>
+      <c r="F2566" t="n">
+        <v>379983</v>
       </c>
     </row>
   </sheetData>

</xml_diff>